<commit_message>
20250916 many minor bug fixes + EFESP
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202509/DEUP.xlsx
+++ b/GUI + Reviews/202509/DEUP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202509\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29980E6C-2E4C-4A6F-AA61-C70866E5F963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD6B4D67-8321-4A9E-BA8D-815DB9C4791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBF0D37C-FA95-4B24-86E4-CFB51FAC83ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E35AD49-54D5-4007-AE6D-533D620505B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="1342">
   <si>
     <t>Name</t>
   </si>
@@ -3963,15 +3963,6 @@
   </si>
   <si>
     <t>DE000A1ML7J1</t>
-  </si>
-  <si>
-    <t>WALLENIUS WILHELMS</t>
-  </si>
-  <si>
-    <t>WAWI-NO</t>
-  </si>
-  <si>
-    <t>NO0010571680</t>
   </si>
   <si>
     <t>WALLENSTAM AB CLSS B</t>
@@ -4373,22 +4364,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2C205764-F33C-4F68-B336-7108B6B85F9A}" name="Universe" displayName="Universe" ref="A1:M438" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:M438" xr:uid="{2C205764-F33C-4F68-B336-7108B6B85F9A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42827501-3EEF-4C74-9D85-3EA60B2A23CE}" name="Universe" displayName="Universe" ref="A1:M437" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:M437" xr:uid="{42827501-3EEF-4C74-9D85-3EA60B2A23CE}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{127A1893-46E2-4787-9523-750BC5724C93}" name="Name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{DC43D4E8-2C7C-40B1-B246-E363B2723170}" name="Ticker" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{4D9C5BD8-A335-4EB8-BD7D-CC1589D77939}" name="ISIN" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D907B536-DF3B-44F7-BA1B-3AF7CF2993C0}" name="MIC" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{FF2A9968-4CC6-4AD1-9A6D-EAA02207AAA3}" name="Currency (Local)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{EEA2DF06-3076-4C3A-9633-BCA8093FF822}" name="Price (EUR) " dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{C1291A5E-B245-4B84-BDE1-452EB5769FBF}" name="NOSH" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{2A389135-50E5-414F-BEE6-16DEC205852C}" name="20 days AVG turnover EUR" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{20FF84F1-0576-4767-B037-DE48E215D1A6}" name="3M AVG Turnover EUR" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{88DBA11D-BDC3-4E95-9BF2-7871C729D87A}" name="3M AVG Turnover USD" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{92809101-A703-4F63-8E75-11E2DC4E86AF}" name="100 Trading Days AVG Turnover EUR" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{454E0CA4-C4B1-4CC5-9B88-E101D9A13A5F}" name="6M AVG Turnover EUR" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{F710ED4B-DCB3-4551-A856-D8109372C500}" name="12M AVG Turnover EUR" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{4399DDBB-F5C2-4E1A-B426-6221AFEF15C9}" name="Name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{5C7AAFBE-E2F2-47BF-9D3D-1B0E3F4E09DE}" name="Ticker" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B395ECEF-C5EB-4FF1-989D-375B68B90F3F}" name="ISIN" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{75154C35-9756-4B62-9989-6E0644DEEF57}" name="MIC" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{820440E2-45AF-4A64-8531-478EDA7A71FF}" name="Currency (Local)" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D26F60C9-D32E-4000-A084-A7FAA85F97F5}" name="Price (EUR) " dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{5C539BA4-837B-4411-B8BE-E096EABCE71D}" name="NOSH" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{09F35518-864E-4042-92FD-220502167CE2}" name="20 days AVG turnover EUR" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{C952FBB7-8F75-4CED-94A2-F8D1EAE53E2A}" name="3M AVG Turnover EUR" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{1B0FFF82-037E-4E22-AB85-C62EB5D2521E}" name="3M AVG Turnover USD" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{887BE6AD-7E68-43F5-B0F8-DFF607892E3A}" name="100 Trading Days AVG Turnover EUR" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{90411CFF-4D83-4D31-BFE1-0CD197FA7C91}" name="6M AVG Turnover EUR" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{54182054-D257-4901-8481-026B727AE7A1}" name="12M AVG Turnover EUR" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4710,8 +4701,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D4CFE3-5779-4A8B-8AAD-D3B73D23D7CF}">
-  <dimension ref="A1:M438"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCEFC7A-FD2A-48B6-8E80-89C3C575F5D8}">
+  <dimension ref="A1:M437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19635,7 +19626,7 @@
         <v>4.9961950000000002</v>
       </c>
       <c r="G364" s="1">
-        <v>700651370</v>
+        <v>700651000</v>
       </c>
       <c r="H364" s="1">
         <v>12233019.293589801</v>
@@ -22209,34 +22200,34 @@
         <v>1311</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="E427" s="1" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="F427" s="1">
-        <v>8.8590959999999992</v>
+        <v>4.0949770000000001</v>
       </c>
       <c r="G427" s="1">
-        <v>423104938</v>
+        <v>591000000</v>
       </c>
       <c r="H427" s="1">
-        <v>4697759.2367837001</v>
+        <v>1691426.8031645601</v>
       </c>
       <c r="I427" s="1">
-        <v>3059566.8202471002</v>
+        <v>2579559.7163915401</v>
       </c>
       <c r="J427" s="1">
-        <v>3548214.3551133401</v>
+        <v>2986509.6415634402</v>
       </c>
       <c r="K427" s="1">
-        <v>3570685.9880774901</v>
+        <v>2687498.6245051599</v>
       </c>
       <c r="L427" s="1">
-        <v>3995049.3127300702</v>
+        <v>2696743.5988780502</v>
       </c>
       <c r="M427" s="1">
-        <v>4248019.3674719203</v>
+        <v>2588804.39360289</v>
       </c>
     </row>
     <row r="428" spans="1:13" x14ac:dyDescent="0.2">
@@ -22250,34 +22241,34 @@
         <v>1314</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>21</v>
+        <v>450</v>
       </c>
       <c r="E428" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F428" s="1">
-        <v>4.0949770000000001</v>
+        <v>24.47</v>
       </c>
       <c r="G428" s="1">
-        <v>591000000</v>
+        <v>591723400</v>
       </c>
       <c r="H428" s="1">
-        <v>1691426.8031645601</v>
+        <v>13675975.676000001</v>
       </c>
       <c r="I428" s="1">
-        <v>2579559.7163915401</v>
+        <v>17546984.039375</v>
       </c>
       <c r="J428" s="1">
-        <v>2986509.6415634402</v>
+        <v>20323623.821837399</v>
       </c>
       <c r="K428" s="1">
-        <v>2687498.6245051599</v>
+        <v>17448989.633699998</v>
       </c>
       <c r="L428" s="1">
-        <v>2696743.5988780502</v>
+        <v>18079612.356079999</v>
       </c>
       <c r="M428" s="1">
-        <v>2588804.39360289</v>
+        <v>17372443.570160601</v>
       </c>
     </row>
     <row r="429" spans="1:13" x14ac:dyDescent="0.2">
@@ -22291,34 +22282,34 @@
         <v>1317</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>450</v>
+        <v>26</v>
       </c>
       <c r="E429" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F429" s="1">
-        <v>24.47</v>
+        <v>22.48</v>
       </c>
       <c r="G429" s="1">
-        <v>591723400</v>
+        <v>232653901</v>
       </c>
       <c r="H429" s="1">
-        <v>13675975.676000001</v>
+        <v>4735172.7560000001</v>
       </c>
       <c r="I429" s="1">
-        <v>17546984.039375</v>
+        <v>5622080.9669696996</v>
       </c>
       <c r="J429" s="1">
-        <v>20323623.821837399</v>
+        <v>6516157.1030495698</v>
       </c>
       <c r="K429" s="1">
-        <v>17448989.633699998</v>
+        <v>6394729.0504999999</v>
       </c>
       <c r="L429" s="1">
-        <v>18079612.356079999</v>
+        <v>9254610.0950393695</v>
       </c>
       <c r="M429" s="1">
-        <v>17372443.570160601</v>
+        <v>8725985.8038235307</v>
       </c>
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.2">
@@ -22332,34 +22323,34 @@
         <v>1320</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E430" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F430" s="1">
-        <v>22.48</v>
+        <v>28.992609999999999</v>
       </c>
       <c r="G430" s="1">
-        <v>232653901</v>
+        <v>259612060</v>
       </c>
       <c r="H430" s="1">
-        <v>4735172.7560000001</v>
+        <v>11920168.570950599</v>
       </c>
       <c r="I430" s="1">
-        <v>5622080.9669696996</v>
+        <v>11161105.453201201</v>
       </c>
       <c r="J430" s="1">
-        <v>6516157.1030495698</v>
+        <v>12939952.3060671</v>
       </c>
       <c r="K430" s="1">
-        <v>6394729.0504999999</v>
+        <v>11885626.662976</v>
       </c>
       <c r="L430" s="1">
-        <v>9254610.0950393695</v>
+        <v>12977887.937461199</v>
       </c>
       <c r="M430" s="1">
-        <v>8725985.8038235307</v>
+        <v>12244769.225099901</v>
       </c>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.2">
@@ -22379,28 +22370,28 @@
         <v>17</v>
       </c>
       <c r="F431" s="1">
-        <v>28.992609999999999</v>
+        <v>36.967880000000001</v>
       </c>
       <c r="G431" s="1">
-        <v>259612060</v>
+        <v>173993260</v>
       </c>
       <c r="H431" s="1">
-        <v>11920168.570950599</v>
+        <v>12050921.7908701</v>
       </c>
       <c r="I431" s="1">
-        <v>11161105.453201201</v>
+        <v>14884502.808193</v>
       </c>
       <c r="J431" s="1">
-        <v>12939952.3060671</v>
+        <v>17239669.889261302</v>
       </c>
       <c r="K431" s="1">
-        <v>11885626.662976</v>
+        <v>15401263.5526441</v>
       </c>
       <c r="L431" s="1">
-        <v>12977887.937461199</v>
+        <v>15566334.6658604</v>
       </c>
       <c r="M431" s="1">
-        <v>12244769.225099901</v>
+        <v>16952344.735906702</v>
       </c>
     </row>
     <row r="432" spans="1:13" x14ac:dyDescent="0.2">
@@ -22414,34 +22405,34 @@
         <v>1326</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="E432" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F432" s="1">
-        <v>36.967880000000001</v>
+        <v>32.18</v>
       </c>
       <c r="G432" s="1">
-        <v>173993260</v>
+        <v>109497696</v>
       </c>
       <c r="H432" s="1">
-        <v>12050921.7908701</v>
+        <v>5515907.0613333303</v>
       </c>
       <c r="I432" s="1">
-        <v>14884502.808193</v>
+        <v>5368013.5598484902</v>
       </c>
       <c r="J432" s="1">
-        <v>17239669.889261302</v>
+        <v>6216493.5740272002</v>
       </c>
       <c r="K432" s="1">
-        <v>15401263.5526441</v>
+        <v>5858576.8919000002</v>
       </c>
       <c r="L432" s="1">
-        <v>15566334.6658604</v>
+        <v>6889833.0951968497</v>
       </c>
       <c r="M432" s="1">
-        <v>16952344.735906702</v>
+        <v>7383607.2848616596</v>
       </c>
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.2">
@@ -22455,34 +22446,34 @@
         <v>1329</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>124</v>
+        <v>21</v>
       </c>
       <c r="E433" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F433" s="1">
-        <v>32.18</v>
+        <v>8.6710820000000002</v>
       </c>
       <c r="G433" s="1">
-        <v>109497696</v>
+        <v>307426900</v>
       </c>
       <c r="H433" s="1">
-        <v>5515907.0613333303</v>
+        <v>1836499.0433165401</v>
       </c>
       <c r="I433" s="1">
-        <v>5368013.5598484902</v>
+        <v>2606761.20408971</v>
       </c>
       <c r="J433" s="1">
-        <v>6216493.5740272002</v>
+        <v>3019567.1725137201</v>
       </c>
       <c r="K433" s="1">
-        <v>5858576.8919000002</v>
+        <v>2984113.2568202498</v>
       </c>
       <c r="L433" s="1">
-        <v>6889833.0951968497</v>
+        <v>3113160.5611916799</v>
       </c>
       <c r="M433" s="1">
-        <v>7383607.2848616596</v>
+        <v>3293136.4136645799</v>
       </c>
     </row>
     <row r="434" spans="1:13" x14ac:dyDescent="0.2">
@@ -22496,34 +22487,34 @@
         <v>1332</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E434" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F434" s="1">
-        <v>8.6710820000000002</v>
+        <v>12.522679999999999</v>
       </c>
       <c r="G434" s="1">
-        <v>307426900</v>
+        <v>1025000200</v>
       </c>
       <c r="H434" s="1">
-        <v>1836499.0433165401</v>
+        <v>8517626.4547434207</v>
       </c>
       <c r="I434" s="1">
-        <v>2606761.20408971</v>
+        <v>15819670.120589999</v>
       </c>
       <c r="J434" s="1">
-        <v>3019567.1725137201</v>
+        <v>18295935.225853201</v>
       </c>
       <c r="K434" s="1">
-        <v>2984113.2568202498</v>
+        <v>15238269.6176915</v>
       </c>
       <c r="L434" s="1">
-        <v>3113160.5611916799</v>
+        <v>14921792.0110755</v>
       </c>
       <c r="M434" s="1">
-        <v>3293136.4136645799</v>
+        <v>14240968.592746001</v>
       </c>
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.2">
@@ -22537,34 +22528,34 @@
         <v>1335</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E435" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F435" s="1">
-        <v>12.522679999999999</v>
+        <v>115.3</v>
       </c>
       <c r="G435" s="1">
-        <v>1025000200</v>
+        <v>238516153</v>
       </c>
       <c r="H435" s="1">
-        <v>8517626.4547434207</v>
+        <v>100347954.28</v>
       </c>
       <c r="I435" s="1">
-        <v>15819670.120589999</v>
+        <v>86599219.077272698</v>
       </c>
       <c r="J435" s="1">
-        <v>18295935.225853201</v>
+        <v>100403840.15354601</v>
       </c>
       <c r="K435" s="1">
-        <v>15238269.6176915</v>
+        <v>90701122.042750001</v>
       </c>
       <c r="L435" s="1">
-        <v>14921792.0110755</v>
+        <v>99599052.755315006</v>
       </c>
       <c r="M435" s="1">
-        <v>14240968.592746001</v>
+        <v>84889715.0388235</v>
       </c>
     </row>
     <row r="436" spans="1:13" x14ac:dyDescent="0.2">
@@ -22578,34 +22569,34 @@
         <v>1338</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="E436" s="1" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="F436" s="1">
-        <v>115.3</v>
+        <v>31.762060000000002</v>
       </c>
       <c r="G436" s="1">
-        <v>238516153</v>
+        <v>254725627</v>
       </c>
       <c r="H436" s="1">
-        <v>100347954.28</v>
+        <v>13416085.7147645</v>
       </c>
       <c r="I436" s="1">
-        <v>86599219.077272698</v>
+        <v>17224241.0786836</v>
       </c>
       <c r="J436" s="1">
-        <v>100403840.15354601</v>
+        <v>19945085.000506099</v>
       </c>
       <c r="K436" s="1">
-        <v>90701122.042750001</v>
+        <v>18205583.758850198</v>
       </c>
       <c r="L436" s="1">
-        <v>99599052.755315006</v>
+        <v>18291811.731256802</v>
       </c>
       <c r="M436" s="1">
-        <v>84889715.0388235</v>
+        <v>16730793.983756</v>
       </c>
     </row>
     <row r="437" spans="1:13" x14ac:dyDescent="0.2">
@@ -22619,74 +22610,33 @@
         <v>1341</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="E437" s="1" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="F437" s="1">
-        <v>31.762060000000002</v>
+        <v>631.35059999999999</v>
       </c>
       <c r="G437" s="1">
-        <v>254725627</v>
+        <v>146355760</v>
       </c>
       <c r="H437" s="1">
-        <v>13416085.7147645</v>
+        <v>135409974.63567799</v>
       </c>
       <c r="I437" s="1">
-        <v>17224241.0786836</v>
+        <v>117164138.64685699</v>
       </c>
       <c r="J437" s="1">
-        <v>19945085.000506099</v>
+        <v>135762120.48838001</v>
       </c>
       <c r="K437" s="1">
-        <v>18205583.758850198</v>
+        <v>151915704.08632499</v>
       </c>
       <c r="L437" s="1">
-        <v>18291811.731256802</v>
+        <v>158401469.820077</v>
       </c>
       <c r="M437" s="1">
-        <v>16730793.983756</v>
-      </c>
-    </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A438" s="1" t="s">
-        <v>1342</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>1343</v>
-      </c>
-      <c r="C438" s="1" t="s">
-        <v>1344</v>
-      </c>
-      <c r="D438" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E438" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F438" s="1">
-        <v>631.35059999999999</v>
-      </c>
-      <c r="G438" s="1">
-        <v>146355760</v>
-      </c>
-      <c r="H438" s="1">
-        <v>135409974.63567799</v>
-      </c>
-      <c r="I438" s="1">
-        <v>117164138.64685699</v>
-      </c>
-      <c r="J438" s="1">
-        <v>135762120.48838001</v>
-      </c>
-      <c r="K438" s="1">
-        <v>151915704.08632499</v>
-      </c>
-      <c r="L438" s="1">
-        <v>158401469.820077</v>
-      </c>
-      <c r="M438" s="1">
         <v>157703770.53286299</v>
       </c>
     </row>

</xml_diff>